<commit_message>
updatating the SRS and SIQ files
</commit_message>
<xml_diff>
--- a/Requirement/REQ_SIQ.xlsx
+++ b/Requirement/REQ_SIQ.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="9140" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="9140"/>
   </bookViews>
   <sheets>
     <sheet name="SIQ" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
   <si>
     <t>Module Name</t>
   </si>
@@ -47,175 +47,189 @@
     <t>SIQ_user_reg_01</t>
   </si>
   <si>
-    <t>Create a new account with Account no. only</t>
-  </si>
-  <si>
     <t>SIQ_user_reg_02</t>
   </si>
   <si>
-    <t>Create a new account with Credit/Debit card only</t>
-  </si>
-  <si>
     <t>SIQ_user_reg_03</t>
   </si>
   <si>
-    <t>Max number of Account input is (20 Digit)</t>
-  </si>
-  <si>
     <t>SIQ_user_reg_04</t>
   </si>
   <si>
-    <t>Max number of Username input (20 Digit)
-Username include numbers
-Username include at least 1 Capital letter
-Username include special char
-Username include spaces
-Username include combination of cap &amp; small characters</t>
-  </si>
-  <si>
     <t>SIQ_user_reg_05</t>
   </si>
   <si>
-    <t>Max number of Password input (20 no)</t>
-  </si>
-  <si>
-    <t>SIQ_user_reg_06</t>
-  </si>
-  <si>
-    <t>Password include at least 1 Capital letter (Mandatory)
+    <t>Admin Features</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>V0</t>
+  </si>
+  <si>
+    <t>18/3/2024</t>
+  </si>
+  <si>
+    <t>Aya  Mostafa</t>
+  </si>
+  <si>
+    <t>Initial draft</t>
+  </si>
+  <si>
+    <t>registration form contains:
+full name
+National ID
+username
+password
+email</t>
+  </si>
+  <si>
+    <t>pasword validity  are:
+Max number of Password input (20 no)
+Password include at least 1 Capital letter (Mandatory)
 Password include special char
 Password  include spaces
 Password include special char
-Password include combination of cap &amp; small</t>
-  </si>
-  <si>
-    <t>SIQ_user_reg_07</t>
-  </si>
-  <si>
-    <t>Error msgs in case of wrong username or password naming conventions</t>
-  </si>
-  <si>
-    <t>SIQ_user_reg_08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E-mail input include capital letters, special character and digits? </t>
-  </si>
-  <si>
-    <t>SIQ_user_reg_09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sending OTP msg to user E-mail </t>
-  </si>
-  <si>
-    <t>SIQ_user_reg_10</t>
-  </si>
-  <si>
-    <t>Confirmation msg in case of complete registration</t>
-  </si>
-  <si>
-    <t>User LogIn</t>
-  </si>
-  <si>
-    <t>SIQ_user_log_11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Redirect to login page </t>
-  </si>
-  <si>
-    <t>SIQ_user_log_12</t>
-  </si>
-  <si>
-    <t>Error msgs in case of wrong username or password</t>
-  </si>
-  <si>
-    <t>SIQ_user_log_13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Max number of account 1 costumer can have </t>
-  </si>
-  <si>
-    <t>SIQ_user_log_15</t>
-  </si>
-  <si>
-    <t>User can change password?</t>
-  </si>
-  <si>
-    <t>SIQ_user_log_16</t>
-  </si>
-  <si>
-    <t>User can view history of all previous transactions?</t>
-  </si>
-  <si>
-    <t>User Transactions</t>
-  </si>
-  <si>
-    <t>SIQ_user_trans_14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Users transactions include :
-1- Balance Enquiry
-2- Fund Transfer
-3- Mini Statment
-</t>
-  </si>
-  <si>
-    <t>Admin Features</t>
-  </si>
-  <si>
-    <t>SIQ_AdminFeatures_01</t>
-  </si>
-  <si>
-    <t>Add Customer
-Edit Customer
-Delete Customer
-Add Account
-Edit Account
-Delete Account
-Reset Customer Password
-View Customer Balance</t>
-  </si>
-  <si>
-    <t>Reset Customer Password</t>
-  </si>
-  <si>
-    <t>SIQ_AdminResetPassword_01</t>
-  </si>
-  <si>
-    <t>Is there a limit of customer password reseting?</t>
-  </si>
-  <si>
-    <t>SIQ_AdminResetPassword_02</t>
-  </si>
-  <si>
-    <t>is the max limit is 3 times each month ?</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>owner</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>V0</t>
-  </si>
-  <si>
-    <t>18/3/2024</t>
-  </si>
-  <si>
-    <t>Aya  Mostafa</t>
-  </si>
-  <si>
-    <t>Initial draft</t>
+Password include combination of cap &amp; small
+The password length must be at least 8 characters.</t>
+  </si>
+  <si>
+    <t>full name validity:
+-numbers are not allowed
+-special character are not allowed
+-allow only characters and spaces
+-not case sensetive</t>
+  </si>
+  <si>
+    <t>after successfully registeration login will not be needed?</t>
+  </si>
+  <si>
+    <t>User Login</t>
+  </si>
+  <si>
+    <t>SIQ_user_log_01</t>
+  </si>
+  <si>
+    <t>SIQ_user_log_02</t>
+  </si>
+  <si>
+    <t>login form contains only :
+-username
+-password
+for all bank accounts</t>
+  </si>
+  <si>
+    <t>SIQ_adminFeatures_01</t>
+  </si>
+  <si>
+    <t>system admin can do:
+Add user
+Delete user
+Add bank Account
+Delete bank Account
+View bank account Balance</t>
+  </si>
+  <si>
+    <t>SIQ_adminFeatures_addUser_02</t>
+  </si>
+  <si>
+    <t>the attributes to add user are the same as per question SIQ_user_reg_01</t>
+  </si>
+  <si>
+    <t>SIQ_adminFeatures_deleteUser_03</t>
+  </si>
+  <si>
+    <t>the attributes to delete user are:
+-National ID</t>
+  </si>
+  <si>
+    <t>SIQ_adminFeatures_addBankAccount_04</t>
+  </si>
+  <si>
+    <t>the attributes to add bank account are:
+- username
+-account number</t>
+  </si>
+  <si>
+    <t>SIQ_adminFeatures_deleteBankAccount_05</t>
+  </si>
+  <si>
+    <t>the attributes to delete bank account are:
+-account number</t>
+  </si>
+  <si>
+    <t>SIQ_adminFeatures_viewBankAccountBalance_06</t>
+  </si>
+  <si>
+    <t>the attributes to view bank account balance are:
+-account number</t>
+  </si>
+  <si>
+    <t>user transaction</t>
+  </si>
+  <si>
+    <t>SIQ_user_balanceEnquiry_01</t>
+  </si>
+  <si>
+    <t>The user can perform transaction as per question 
+SIQ_user_transaction_04</t>
+  </si>
+  <si>
+    <t>SIQ_user_balanceEnquiry_02</t>
+  </si>
+  <si>
+    <t>The user can view account details as per question  SIQ_user_bankAccount_03</t>
+  </si>
+  <si>
+    <t>SIQ_user_bankAccount_03</t>
+  </si>
+  <si>
+    <t>bank account attributes are only:
+-bank account Balance
+-bank account Transactions History 
+-bank account number</t>
+  </si>
+  <si>
+    <t>SIQ_user_transactions_04</t>
+  </si>
+  <si>
+    <t>Each Transaction attributes are only:
+-source account
+-destination account
+-Trans ID
+- Amount
+-Type(withdraw /deposit)
+-bank account number</t>
+  </si>
+  <si>
+    <t>System Technology</t>
+  </si>
+  <si>
+    <t>SIQ_sys_technology_01</t>
+  </si>
+  <si>
+    <t>system will have web interface only?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>all user banking accounts are connected so the user will have one username and password
+ to use for access all his bank accounts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -255,8 +269,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,18 +291,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -290,37 +322,157 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,21 +901,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="23.7265625" customWidth="1"/>
     <col min="2" max="2" width="41.6328125" customWidth="1"/>
-    <col min="3" max="3" width="82.453125" customWidth="1"/>
-    <col min="4" max="6" width="12.6328125" customWidth="1"/>
+    <col min="3" max="3" width="70.1796875" customWidth="1"/>
+    <col min="4" max="4" width="12.6328125" customWidth="1"/>
+    <col min="5" max="5" width="46.08984375" customWidth="1"/>
+    <col min="6" max="6" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -788,304 +942,317 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
-    </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="7" t="s">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+    </row>
+    <row r="2" spans="1:26" s="9" customFormat="1" ht="99" customHeight="1" thickBot="1">
+      <c r="A2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="1:26" s="9" customFormat="1" ht="110.5" customHeight="1" thickBot="1">
+      <c r="A3" s="22"/>
+      <c r="B3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A3" s="8"/>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="12"/>
+    </row>
+    <row r="4" spans="1:26" s="9" customFormat="1" ht="134.5" customHeight="1" thickBot="1">
+      <c r="A4" s="22"/>
+      <c r="B4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="12"/>
+    </row>
+    <row r="5" spans="1:26" s="9" customFormat="1" ht="94" customHeight="1" thickBot="1">
+      <c r="A5" s="22"/>
+      <c r="B5" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A4" s="8"/>
-      <c r="B4" s="3" t="s">
+      <c r="C5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="13"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="12"/>
+    </row>
+    <row r="6" spans="1:26" s="9" customFormat="1" ht="44" customHeight="1" thickBot="1">
+      <c r="A6" s="23"/>
+      <c r="B6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="27"/>
+    </row>
+    <row r="7" spans="1:26" s="8" customFormat="1" ht="45" customHeight="1" thickBot="1">
+      <c r="A7" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="16"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="29"/>
+    </row>
+    <row r="8" spans="1:26" s="8" customFormat="1" ht="78" customHeight="1" thickBot="1">
+      <c r="A8" s="25"/>
+      <c r="B8" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="16"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="29"/>
+    </row>
+    <row r="9" spans="1:26" s="9" customFormat="1" ht="98.5" customHeight="1" thickBot="1">
+      <c r="A9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A12" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="3" t="s">
+      <c r="B9" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="8"/>
-      <c r="B13" s="3" t="s">
+      <c r="D9" s="13"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="27"/>
+    </row>
+    <row r="10" spans="1:26" s="9" customFormat="1" ht="41" customHeight="1" thickBot="1">
+      <c r="A10" s="22"/>
+      <c r="B10" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C10" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A14" s="8"/>
-      <c r="B14" s="3" t="s">
+      <c r="D10" s="13"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="27"/>
+    </row>
+    <row r="11" spans="1:26" s="9" customFormat="1" ht="46" customHeight="1" thickBot="1">
+      <c r="A11" s="22"/>
+      <c r="B11" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C11" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A15" s="8"/>
-      <c r="B15" s="3" t="s">
+      <c r="D11" s="13"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="27"/>
+    </row>
+    <row r="12" spans="1:26" s="9" customFormat="1" ht="57.5" customHeight="1" thickBot="1">
+      <c r="A12" s="22"/>
+      <c r="B12" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C12" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A16" s="8"/>
-      <c r="B16" s="3" t="s">
+      <c r="D12" s="13"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="27"/>
+    </row>
+    <row r="13" spans="1:26" s="9" customFormat="1" ht="56.5" customHeight="1" thickBot="1">
+      <c r="A13" s="22"/>
+      <c r="B13" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C13" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" ht="4" customHeight="1">
-      <c r="A17" s="8"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A18" s="3" t="s">
+      <c r="D13" s="13"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="27"/>
+    </row>
+    <row r="14" spans="1:26" s="9" customFormat="1" ht="44.5" customHeight="1" thickBot="1">
+      <c r="A14" s="23"/>
+      <c r="B14" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="C14" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="D14" s="13"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="27"/>
+    </row>
+    <row r="15" spans="1:26" s="8" customFormat="1" ht="53" customHeight="1" thickBot="1">
+      <c r="A15" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="4"/>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A19" s="3" t="s">
+      <c r="B15" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C15" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="D15" s="16"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="29"/>
+    </row>
+    <row r="16" spans="1:26" s="8" customFormat="1" ht="31.5" customHeight="1" thickBot="1">
+      <c r="A16" s="19"/>
+      <c r="B16" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="4"/>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A20" s="10" t="s">
+      <c r="C16" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="D16" s="16"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="29"/>
+    </row>
+    <row r="17" spans="1:8" s="8" customFormat="1" ht="59" customHeight="1" thickBot="1">
+      <c r="A17" s="19"/>
+      <c r="B17" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C17" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
-      <c r="G20" s="4"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A21" s="8"/>
-      <c r="B21" s="3" t="s">
+      <c r="D17" s="16"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="29"/>
+    </row>
+    <row r="18" spans="1:8" s="8" customFormat="1" ht="106" customHeight="1" thickBot="1">
+      <c r="A18" s="20"/>
+      <c r="B18" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C18" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="4"/>
-      <c r="G21" s="4"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A22" s="4"/>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A23" s="4"/>
-      <c r="G23" s="4"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="29"/>
+    </row>
+    <row r="19" spans="1:8" s="9" customFormat="1" ht="25.5" customHeight="1" thickBot="1">
+      <c r="A19" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="15"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="27"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="24" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="25" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="26" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:8" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -2053,19 +2220,20 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="A12:A17"/>
-    <mergeCell ref="A20:A21"/>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A14"/>
+    <mergeCell ref="A15:A18"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D21">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D20">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2073,7 +2241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -2084,32 +2252,32 @@
     <col min="4" max="4" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="11" customFormat="1" ht="26.5" customHeight="1">
-      <c r="A1" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:4" s="7" customFormat="1" ht="26.5" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>53</v>
+      <c r="C1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set the time plan for design phase
</commit_message>
<xml_diff>
--- a/Requirement/REQ_SIQ.xlsx
+++ b/Requirement/REQ_SIQ.xlsx
@@ -661,6 +661,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
@@ -670,6 +679,8 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -679,9 +690,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -694,25 +702,17 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1154,8 +1154,8 @@
   </sheetPr>
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:D28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -1213,7 +1213,7 @@
       <c r="Z1" s="9"/>
     </row>
     <row r="2" spans="1:26" s="4" customFormat="1" ht="84">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="41" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -1249,7 +1249,7 @@
       <c r="Z2" s="17"/>
     </row>
     <row r="3" spans="1:26" s="4" customFormat="1" ht="112">
-      <c r="A3" s="36"/>
+      <c r="A3" s="39"/>
       <c r="B3" s="12" t="s">
         <v>10</v>
       </c>
@@ -1283,7 +1283,7 @@
       <c r="Z3" s="17"/>
     </row>
     <row r="4" spans="1:26" s="4" customFormat="1" ht="126">
-      <c r="A4" s="36"/>
+      <c r="A4" s="39"/>
       <c r="B4" s="12" t="s">
         <v>11</v>
       </c>
@@ -1319,7 +1319,7 @@
       <c r="Z4" s="17"/>
     </row>
     <row r="5" spans="1:26" s="4" customFormat="1" ht="98">
-      <c r="A5" s="36"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="12" t="s">
         <v>12</v>
       </c>
@@ -1353,7 +1353,7 @@
       <c r="Z5" s="20"/>
     </row>
     <row r="6" spans="1:26" s="4" customFormat="1" ht="14">
-      <c r="A6" s="36"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="12" t="s">
         <v>13</v>
       </c>
@@ -1387,7 +1387,7 @@
       <c r="Z6" s="22"/>
     </row>
     <row r="7" spans="1:26" s="3" customFormat="1" ht="84">
-      <c r="A7" s="36"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="12" t="s">
         <v>42</v>
       </c>
@@ -1421,7 +1421,7 @@
       <c r="Z7" s="22"/>
     </row>
     <row r="8" spans="1:26" s="3" customFormat="1" ht="28">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="42" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="23" t="s">
@@ -1457,7 +1457,7 @@
       <c r="Z8" s="28"/>
     </row>
     <row r="9" spans="1:26" s="4" customFormat="1" ht="56">
-      <c r="A9" s="37"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="23" t="s">
         <v>25</v>
       </c>
@@ -1491,7 +1491,7 @@
       <c r="Z9" s="29"/>
     </row>
     <row r="10" spans="1:26" s="4" customFormat="1" ht="84">
-      <c r="A10" s="40" t="s">
+      <c r="A10" s="45" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="12" t="s">
@@ -1527,7 +1527,7 @@
       <c r="Z10" s="17"/>
     </row>
     <row r="11" spans="1:26" s="4" customFormat="1" ht="14">
-      <c r="A11" s="36"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="12" t="s">
         <v>29</v>
       </c>
@@ -1561,7 +1561,7 @@
       <c r="Z11" s="17"/>
     </row>
     <row r="12" spans="1:26" s="4" customFormat="1" ht="28">
-      <c r="A12" s="36"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="12" t="s">
         <v>31</v>
       </c>
@@ -1595,7 +1595,7 @@
       <c r="Z12" s="17"/>
     </row>
     <row r="13" spans="1:26" s="4" customFormat="1" ht="42">
-      <c r="A13" s="36"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="12" t="s">
         <v>33</v>
       </c>
@@ -1629,7 +1629,7 @@
       <c r="Z13" s="17"/>
     </row>
     <row r="14" spans="1:26" s="4" customFormat="1" ht="28">
-      <c r="A14" s="36"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="12" t="s">
         <v>35</v>
       </c>
@@ -1663,7 +1663,7 @@
       <c r="Z14" s="17"/>
     </row>
     <row r="15" spans="1:26" s="3" customFormat="1" ht="28">
-      <c r="A15" s="36"/>
+      <c r="A15" s="39"/>
       <c r="B15" s="12" t="s">
         <v>37</v>
       </c>
@@ -1697,7 +1697,7 @@
       <c r="Z15" s="17"/>
     </row>
     <row r="16" spans="1:26" s="3" customFormat="1" ht="70">
-      <c r="A16" s="37"/>
+      <c r="A16" s="40"/>
       <c r="B16" s="12" t="s">
         <v>45</v>
       </c>
@@ -1730,8 +1730,8 @@
       <c r="Y16" s="17"/>
       <c r="Z16" s="17"/>
     </row>
-    <row r="17" spans="1:26" s="3" customFormat="1" ht="70">
-      <c r="A17" s="42"/>
+    <row r="17" spans="1:26" s="3" customFormat="1" ht="111.5" customHeight="1">
+      <c r="A17" s="47"/>
       <c r="B17" s="30" t="s">
         <v>67</v>
       </c>
@@ -1765,7 +1765,7 @@
       <c r="Z17" s="33"/>
     </row>
     <row r="18" spans="1:26" s="3" customFormat="1" ht="126">
-      <c r="A18" s="36"/>
+      <c r="A18" s="39"/>
       <c r="B18" s="30" t="s">
         <v>48</v>
       </c>
@@ -1801,17 +1801,17 @@
       <c r="Z18" s="33"/>
     </row>
     <row r="19" spans="1:26" s="4" customFormat="1" ht="12.5" customHeight="1">
-      <c r="A19" s="36"/>
-      <c r="B19" s="48" t="s">
+      <c r="A19" s="39"/>
+      <c r="B19" s="55" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="43" t="s">
+      <c r="D19" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="E19" s="35"/>
+      <c r="E19" s="38"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -1835,11 +1835,11 @@
       <c r="Z19" s="5"/>
     </row>
     <row r="20" spans="1:26" ht="12.5" customHeight="1">
-      <c r="A20" s="36"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="36"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="39"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -1862,12 +1862,12 @@
       <c r="Y20" s="5"/>
       <c r="Z20" s="5"/>
     </row>
-    <row r="21" spans="1:26" ht="12.5">
-      <c r="A21" s="36"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="36"/>
+    <row r="21" spans="1:26" ht="28.5" customHeight="1">
+      <c r="A21" s="39"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="39"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
@@ -1891,17 +1891,17 @@
       <c r="Z21" s="5"/>
     </row>
     <row r="22" spans="1:26" ht="12.5">
-      <c r="A22" s="36"/>
-      <c r="B22" s="48" t="s">
+      <c r="A22" s="39"/>
+      <c r="B22" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="50" t="s">
+      <c r="C22" s="52" t="s">
         <v>53</v>
       </c>
       <c r="D22" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="53"/>
+      <c r="E22" s="43"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -1925,11 +1925,11 @@
       <c r="Z22" s="5"/>
     </row>
     <row r="23" spans="1:26" ht="12.5">
-      <c r="A23" s="36"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="51"/>
+      <c r="A23" s="39"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="53"/>
       <c r="D23" s="57"/>
-      <c r="E23" s="53"/>
+      <c r="E23" s="43"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
@@ -1953,11 +1953,11 @@
       <c r="Z23" s="5"/>
     </row>
     <row r="24" spans="1:26" ht="12.5">
-      <c r="A24" s="36"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="51"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="53"/>
       <c r="D24" s="57"/>
-      <c r="E24" s="53"/>
+      <c r="E24" s="43"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
@@ -1981,11 +1981,11 @@
       <c r="Z24" s="5"/>
     </row>
     <row r="25" spans="1:26" ht="12.5">
-      <c r="A25" s="36"/>
-      <c r="B25" s="36"/>
-      <c r="C25" s="51"/>
+      <c r="A25" s="39"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="53"/>
       <c r="D25" s="57"/>
-      <c r="E25" s="53"/>
+      <c r="E25" s="43"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
@@ -2009,11 +2009,11 @@
       <c r="Z25" s="5"/>
     </row>
     <row r="26" spans="1:26" ht="12.5">
-      <c r="A26" s="36"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="51"/>
+      <c r="A26" s="39"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="53"/>
       <c r="D26" s="57"/>
-      <c r="E26" s="53"/>
+      <c r="E26" s="43"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
@@ -2037,11 +2037,11 @@
       <c r="Z26" s="5"/>
     </row>
     <row r="27" spans="1:26" ht="12.5">
-      <c r="A27" s="36"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="51"/>
+      <c r="A27" s="39"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="53"/>
       <c r="D27" s="57"/>
-      <c r="E27" s="53"/>
+      <c r="E27" s="43"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
@@ -2065,11 +2065,11 @@
       <c r="Z27" s="5"/>
     </row>
     <row r="28" spans="1:26" ht="12.5">
-      <c r="A28" s="36"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="52"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="54"/>
       <c r="D28" s="58"/>
-      <c r="E28" s="54"/>
+      <c r="E28" s="44"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
@@ -2093,17 +2093,17 @@
       <c r="Z28" s="5"/>
     </row>
     <row r="29" spans="1:26" ht="12.5">
-      <c r="A29" s="36"/>
-      <c r="B29" s="41" t="s">
+      <c r="A29" s="39"/>
+      <c r="B29" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="44" t="s">
+      <c r="C29" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="49" t="s">
+      <c r="D29" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="E29" s="35"/>
+      <c r="E29" s="38"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
@@ -2127,11 +2127,11 @@
       <c r="Z29" s="5"/>
     </row>
     <row r="30" spans="1:26" ht="12.5">
-      <c r="A30" s="36"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
@@ -2155,11 +2155,11 @@
       <c r="Z30" s="5"/>
     </row>
     <row r="31" spans="1:26" ht="12.5">
-      <c r="A31" s="36"/>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
+      <c r="A31" s="39"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
@@ -2183,11 +2183,11 @@
       <c r="Z31" s="5"/>
     </row>
     <row r="32" spans="1:26" ht="12.5">
-      <c r="A32" s="36"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
+      <c r="A32" s="39"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
@@ -2211,11 +2211,11 @@
       <c r="Z32" s="5"/>
     </row>
     <row r="33" spans="1:26" ht="12.5">
-      <c r="A33" s="36"/>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -2239,11 +2239,11 @@
       <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:26" ht="12.5">
-      <c r="A34" s="36"/>
-      <c r="B34" s="36"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
+      <c r="A34" s="39"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -2267,11 +2267,11 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" ht="12.5">
-      <c r="A35" s="36"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
+      <c r="A35" s="39"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>

</xml_diff>

<commit_message>
Adding the balance deletion criteria to REQ_SIQ file
</commit_message>
<xml_diff>
--- a/Requirement/REQ_SIQ.xlsx
+++ b/Requirement/REQ_SIQ.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="75">
   <si>
     <t>Module Name</t>
   </si>
@@ -130,22 +130,13 @@
 -National ID</t>
   </si>
   <si>
-    <t>SIQ_adminFeatures_addBankAccount_04</t>
-  </si>
-  <si>
     <t>the attributes to add bank account are:
 - username
 -account number</t>
   </si>
   <si>
-    <t>SIQ_adminFeatures_deleteBankAccount_05</t>
-  </si>
-  <si>
     <t>the attributes to delete bank account are:
 -account number</t>
-  </si>
-  <si>
-    <t>SIQ_adminFeatures_viewBankAccountBalance_06</t>
   </si>
   <si>
     <t>the attributes to view bank account balance are:
@@ -196,9 +187,6 @@
     <t>all user banking accounts are connected so the user will have one username and password to use for access all his bank accounts</t>
   </si>
   <si>
-    <t>SIQ_adminFeatures_accountNumField_07</t>
-  </si>
-  <si>
     <t>account number field validity:
 -shouldn't be blank
 -allow numbers only
@@ -298,6 +286,30 @@
   </si>
   <si>
     <t>Yes, you can exclude "balance after transaction"</t>
+  </si>
+  <si>
+    <t>SIQ_adminFeatures_deleteBankAccount_06</t>
+  </si>
+  <si>
+    <t>Admin can delete user if and only if all his accounts balance values is equal to zero.</t>
+  </si>
+  <si>
+    <t>Admin can delete bank account if and only if it's balance value iseqal to zero.</t>
+  </si>
+  <si>
+    <t>SIQ_adminFeatures_deleteUser_04</t>
+  </si>
+  <si>
+    <t>SIQ_adminFeatures_addBankAccount_05</t>
+  </si>
+  <si>
+    <t>SIQ_adminFeatures_deleteBankAccount_07</t>
+  </si>
+  <si>
+    <t>SIQ_adminFeatures_viewBankAccountBalance_08</t>
+  </si>
+  <si>
+    <t>SIQ_adminFeatures_accountNumField_09</t>
   </si>
 </sst>
 </file>
@@ -1152,17 +1164,17 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="23.7265625" customWidth="1"/>
     <col min="2" max="2" width="41.6328125" customWidth="1"/>
-    <col min="3" max="3" width="70.1796875" customWidth="1"/>
+    <col min="3" max="3" width="72.08984375" customWidth="1"/>
     <col min="4" max="4" width="12.6328125" customWidth="1"/>
     <col min="5" max="5" width="46.08984375" customWidth="1"/>
     <col min="6" max="6" width="12.6328125" customWidth="1"/>
@@ -1223,7 +1235,7 @@
         <v>21</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="14"/>
@@ -1254,10 +1266,10 @@
         <v>10</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E3" s="18"/>
       <c r="F3" s="14"/>
@@ -1288,13 +1300,13 @@
         <v>11</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
@@ -1324,10 +1336,10 @@
         <v>12</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E5" s="18"/>
       <c r="F5" s="14"/>
@@ -1361,7 +1373,7 @@
         <v>22</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E6" s="18"/>
       <c r="F6" s="14"/>
@@ -1389,13 +1401,13 @@
     <row r="7" spans="1:26" s="3" customFormat="1" ht="84">
       <c r="A7" s="39"/>
       <c r="B7" s="12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E7" s="18"/>
       <c r="F7" s="14"/>
@@ -1428,10 +1440,10 @@
         <v>24</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="26"/>
@@ -1465,7 +1477,7 @@
         <v>26</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="26"/>
@@ -1501,7 +1513,7 @@
         <v>28</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E10" s="18"/>
       <c r="F10" s="15"/>
@@ -1535,7 +1547,7 @@
         <v>30</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E11" s="18"/>
       <c r="F11" s="15"/>
@@ -1566,11 +1578,9 @@
         <v>31</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="12" t="s">
         <v>68</v>
       </c>
+      <c r="D12" s="12"/>
       <c r="E12" s="18"/>
       <c r="F12" s="15"/>
       <c r="G12" s="14"/>
@@ -1594,16 +1604,16 @@
       <c r="Y12" s="17"/>
       <c r="Z12" s="17"/>
     </row>
-    <row r="13" spans="1:26" s="4" customFormat="1" ht="42">
+    <row r="13" spans="1:26" s="4" customFormat="1" ht="28">
       <c r="A13" s="39"/>
       <c r="B13" s="12" t="s">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="15"/>
@@ -1628,16 +1638,16 @@
       <c r="Y13" s="17"/>
       <c r="Z13" s="17"/>
     </row>
-    <row r="14" spans="1:26" s="4" customFormat="1" ht="28">
+    <row r="14" spans="1:26" s="4" customFormat="1" ht="42">
       <c r="A14" s="39"/>
       <c r="B14" s="12" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="15"/>
@@ -1662,17 +1672,15 @@
       <c r="Y14" s="17"/>
       <c r="Z14" s="17"/>
     </row>
-    <row r="15" spans="1:26" s="3" customFormat="1" ht="28">
+    <row r="15" spans="1:26" s="4" customFormat="1" ht="14">
       <c r="A15" s="39"/>
       <c r="B15" s="12" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>68</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="D15" s="12"/>
       <c r="E15" s="18"/>
       <c r="F15" s="15"/>
       <c r="G15" s="14"/>
@@ -1696,16 +1704,16 @@
       <c r="Y15" s="17"/>
       <c r="Z15" s="17"/>
     </row>
-    <row r="16" spans="1:26" s="3" customFormat="1" ht="70">
-      <c r="A16" s="40"/>
+    <row r="16" spans="1:26" s="4" customFormat="1" ht="28">
+      <c r="A16" s="39"/>
       <c r="B16" s="12" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E16" s="18"/>
       <c r="F16" s="15"/>
@@ -1730,144 +1738,156 @@
       <c r="Y16" s="17"/>
       <c r="Z16" s="17"/>
     </row>
-    <row r="17" spans="1:26" s="3" customFormat="1" ht="111.5" customHeight="1">
-      <c r="A17" s="47"/>
-      <c r="B17" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="C17" s="31" t="s">
+    <row r="17" spans="1:26" s="3" customFormat="1" ht="28">
+      <c r="A17" s="39"/>
+      <c r="B17" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="18"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+      <c r="O17" s="17"/>
+      <c r="P17" s="17"/>
+      <c r="Q17" s="17"/>
+      <c r="R17" s="17"/>
+      <c r="S17" s="17"/>
+      <c r="T17" s="17"/>
+      <c r="U17" s="17"/>
+      <c r="V17" s="17"/>
+      <c r="W17" s="17"/>
+      <c r="X17" s="17"/>
+      <c r="Y17" s="17"/>
+      <c r="Z17" s="17"/>
+    </row>
+    <row r="18" spans="1:26" s="3" customFormat="1" ht="70">
+      <c r="A18" s="40"/>
+      <c r="B18" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E18" s="18"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="17"/>
+      <c r="R18" s="17"/>
+      <c r="S18" s="17"/>
+      <c r="T18" s="17"/>
+      <c r="U18" s="17"/>
+      <c r="V18" s="17"/>
+      <c r="W18" s="17"/>
+      <c r="X18" s="17"/>
+      <c r="Y18" s="17"/>
+      <c r="Z18" s="17"/>
+    </row>
+    <row r="19" spans="1:26" s="3" customFormat="1" ht="111.5" customHeight="1">
+      <c r="A19" s="47"/>
+      <c r="B19" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="33"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
+      <c r="O19" s="33"/>
+      <c r="P19" s="33"/>
+      <c r="Q19" s="33"/>
+      <c r="R19" s="33"/>
+      <c r="S19" s="33"/>
+      <c r="T19" s="33"/>
+      <c r="U19" s="33"/>
+      <c r="V19" s="33"/>
+      <c r="W19" s="33"/>
+      <c r="X19" s="33"/>
+      <c r="Y19" s="33"/>
+      <c r="Z19" s="33"/>
+    </row>
+    <row r="20" spans="1:26" s="3" customFormat="1" ht="126">
+      <c r="A20" s="39"/>
+      <c r="B20" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="33"/>
+      <c r="L20" s="33"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="33"/>
+      <c r="P20" s="33"/>
+      <c r="Q20" s="33"/>
+      <c r="R20" s="33"/>
+      <c r="S20" s="33"/>
+      <c r="T20" s="33"/>
+      <c r="U20" s="33"/>
+      <c r="V20" s="33"/>
+      <c r="W20" s="33"/>
+      <c r="X20" s="33"/>
+      <c r="Y20" s="33"/>
+      <c r="Z20" s="33"/>
+    </row>
+    <row r="21" spans="1:26" s="4" customFormat="1" ht="12.5" customHeight="1">
+      <c r="A21" s="39"/>
+      <c r="B21" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
-      <c r="L17" s="33"/>
-      <c r="M17" s="33"/>
-      <c r="N17" s="33"/>
-      <c r="O17" s="33"/>
-      <c r="P17" s="33"/>
-      <c r="Q17" s="33"/>
-      <c r="R17" s="33"/>
-      <c r="S17" s="33"/>
-      <c r="T17" s="33"/>
-      <c r="U17" s="33"/>
-      <c r="V17" s="33"/>
-      <c r="W17" s="33"/>
-      <c r="X17" s="33"/>
-      <c r="Y17" s="33"/>
-      <c r="Z17" s="33"/>
-    </row>
-    <row r="18" spans="1:26" s="3" customFormat="1" ht="126">
-      <c r="A18" s="39"/>
-      <c r="B18" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
-      <c r="L18" s="33"/>
-      <c r="M18" s="33"/>
-      <c r="N18" s="33"/>
-      <c r="O18" s="33"/>
-      <c r="P18" s="33"/>
-      <c r="Q18" s="33"/>
-      <c r="R18" s="33"/>
-      <c r="S18" s="33"/>
-      <c r="T18" s="33"/>
-      <c r="U18" s="33"/>
-      <c r="V18" s="33"/>
-      <c r="W18" s="33"/>
-      <c r="X18" s="33"/>
-      <c r="Y18" s="33"/>
-      <c r="Z18" s="33"/>
-    </row>
-    <row r="19" spans="1:26" s="4" customFormat="1" ht="12.5" customHeight="1">
-      <c r="A19" s="39"/>
-      <c r="B19" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="35" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="38"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="5"/>
-      <c r="U19" s="5"/>
-      <c r="V19" s="5"/>
-      <c r="W19" s="5"/>
-      <c r="X19" s="5"/>
-      <c r="Y19" s="5"/>
-      <c r="Z19" s="5"/>
-    </row>
-    <row r="20" spans="1:26" ht="12.5" customHeight="1">
-      <c r="A20" s="39"/>
-      <c r="B20" s="39"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
-      <c r="T20" s="5"/>
-      <c r="U20" s="5"/>
-      <c r="V20" s="5"/>
-      <c r="W20" s="5"/>
-      <c r="X20" s="5"/>
-      <c r="Y20" s="5"/>
-      <c r="Z20" s="5"/>
-    </row>
-    <row r="21" spans="1:26" ht="28.5" customHeight="1">
-      <c r="A21" s="39"/>
-      <c r="B21" s="40"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="39"/>
+      <c r="D21" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" s="38"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
@@ -1890,18 +1910,12 @@
       <c r="Y21" s="5"/>
       <c r="Z21" s="5"/>
     </row>
-    <row r="22" spans="1:26" ht="12.5">
+    <row r="22" spans="1:26" ht="12.5" customHeight="1">
       <c r="A22" s="39"/>
-      <c r="B22" s="55" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="52" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="56" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="43"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="39"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -1924,12 +1938,12 @@
       <c r="Y22" s="5"/>
       <c r="Z22" s="5"/>
     </row>
-    <row r="23" spans="1:26" ht="12.5">
+    <row r="23" spans="1:26" ht="28.5" customHeight="1">
       <c r="A23" s="39"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="43"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="39"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
@@ -1954,9 +1968,15 @@
     </row>
     <row r="24" spans="1:26" ht="12.5">
       <c r="A24" s="39"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="57"/>
+      <c r="B24" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="56" t="s">
+        <v>64</v>
+      </c>
       <c r="E24" s="43"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -2066,10 +2086,10 @@
     </row>
     <row r="28" spans="1:26" ht="12.5">
       <c r="A28" s="39"/>
-      <c r="B28" s="40"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="58"/>
-      <c r="E28" s="44"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="43"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
@@ -2094,16 +2114,10 @@
     </row>
     <row r="29" spans="1:26" ht="12.5">
       <c r="A29" s="39"/>
-      <c r="B29" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="48" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" s="38"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="43"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
@@ -2128,10 +2142,10 @@
     </row>
     <row r="30" spans="1:26" ht="12.5">
       <c r="A30" s="39"/>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="44"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
@@ -2156,10 +2170,16 @@
     </row>
     <row r="31" spans="1:26" ht="12.5">
       <c r="A31" s="39"/>
-      <c r="B31" s="39"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
+      <c r="B31" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="38"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
@@ -2216,27 +2236,27 @@
       <c r="C33" s="39"/>
       <c r="D33" s="39"/>
       <c r="E33" s="39"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
-      <c r="S33" s="1"/>
-      <c r="T33" s="1"/>
-      <c r="U33" s="1"/>
-      <c r="V33" s="1"/>
-      <c r="W33" s="1"/>
-      <c r="X33" s="1"/>
-      <c r="Y33" s="1"/>
-      <c r="Z33" s="1"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="5"/>
+      <c r="W33" s="5"/>
+      <c r="X33" s="5"/>
+      <c r="Y33" s="5"/>
+      <c r="Z33" s="5"/>
     </row>
     <row r="34" spans="1:26" ht="12.5">
       <c r="A34" s="39"/>
@@ -2244,34 +2264,34 @@
       <c r="C34" s="39"/>
       <c r="D34" s="39"/>
       <c r="E34" s="39"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
-      <c r="S34" s="1"/>
-      <c r="T34" s="1"/>
-      <c r="U34" s="1"/>
-      <c r="V34" s="1"/>
-      <c r="W34" s="1"/>
-      <c r="X34" s="1"/>
-      <c r="Y34" s="1"/>
-      <c r="Z34" s="1"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="5"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="5"/>
+      <c r="W34" s="5"/>
+      <c r="X34" s="5"/>
+      <c r="Y34" s="5"/>
+      <c r="Z34" s="5"/>
     </row>
     <row r="35" spans="1:26" ht="12.5">
       <c r="A35" s="39"/>
-      <c r="B35" s="40"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="40"/>
-      <c r="E35" s="40"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -2294,8 +2314,62 @@
       <c r="Y35" s="1"/>
       <c r="Z35" s="1"/>
     </row>
-    <row r="36" spans="1:26" ht="15.75" customHeight="1"/>
-    <row r="37" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="36" spans="1:26" ht="12.5">
+      <c r="A36" s="39"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+      <c r="Y36" s="1"/>
+      <c r="Z36" s="1"/>
+    </row>
+    <row r="37" spans="1:26" ht="12.5">
+      <c r="A37" s="39"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="1"/>
+      <c r="Z37" s="1"/>
+    </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="39" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="40" spans="1:26" ht="15.75" customHeight="1"/>
@@ -3258,26 +3332,28 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
+    <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="D19:D21"/>
-    <mergeCell ref="E29:E35"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E31:E37"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E19:E28"/>
-    <mergeCell ref="A10:A16"/>
-    <mergeCell ref="B29:B35"/>
-    <mergeCell ref="A17:A35"/>
-    <mergeCell ref="C29:C35"/>
-    <mergeCell ref="C19:C21"/>
-    <mergeCell ref="C22:C28"/>
-    <mergeCell ref="B22:B28"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="D29:D35"/>
-    <mergeCell ref="D22:D28"/>
+    <mergeCell ref="E21:E30"/>
+    <mergeCell ref="A10:A18"/>
+    <mergeCell ref="B31:B37"/>
+    <mergeCell ref="A19:A37"/>
+    <mergeCell ref="C31:C37"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="C24:C30"/>
+    <mergeCell ref="B24:B30"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="D31:D37"/>
+    <mergeCell ref="D24:D30"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D19">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D2:D21">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3317,7 +3393,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -3331,21 +3407,21 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" t="s">
         <v>57</v>
-      </c>
-      <c r="B3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B4" s="34">
         <v>45508</v>
@@ -3354,21 +3430,21 @@
         <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update revision report table for REQ_SIQ file
</commit_message>
<xml_diff>
--- a/Requirement/REQ_SIQ.xlsx
+++ b/Requirement/REQ_SIQ.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="9140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="9140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SIQ" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="78">
   <si>
     <t>Module Name</t>
   </si>
@@ -310,6 +310,15 @@
   </si>
   <si>
     <t>SIQ_adminFeatures_accountNumField_09</t>
+  </si>
+  <si>
+    <t>V3.1</t>
+  </si>
+  <si>
+    <t>25/4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adding the balance deletion criteria </t>
   </si>
 </sst>
 </file>
@@ -1166,8 +1175,8 @@
   </sheetPr>
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -1580,7 +1589,9 @@
       <c r="C12" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="12"/>
+      <c r="D12" s="12" t="s">
+        <v>64</v>
+      </c>
       <c r="E12" s="18"/>
       <c r="F12" s="15"/>
       <c r="G12" s="14"/>
@@ -1680,7 +1691,9 @@
       <c r="C15" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="12"/>
+      <c r="D15" s="12" t="s">
+        <v>64</v>
+      </c>
       <c r="E15" s="18"/>
       <c r="F15" s="15"/>
       <c r="G15" s="14"/>
@@ -3364,10 +3377,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -3447,6 +3460,20 @@
         <v>59</v>
       </c>
     </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>